<commit_message>
Add forms and actions for grunt adbpush-tables-rowlevelaccessdemo  (incomplete)
</commit_message>
<xml_diff>
--- a/app/config/tables/geoweather/forms/geoweather/geoweather.xlsx
+++ b/app/config/tables/geoweather/forms/geoweather/geoweather.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\geoweather\forms\geoweather\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="5446" yWindow="275" windowWidth="25606" windowHeight="16063" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="settings" sheetId="3" r:id="rId2"/>
-    <sheet name="choices" sheetId="4" r:id="rId3"/>
+    <sheet name="properties" sheetId="6" r:id="rId2"/>
+    <sheet name="queries" sheetId="5" r:id="rId3"/>
+    <sheet name="settings" sheetId="3" r:id="rId4"/>
+    <sheet name="choices" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
   <si>
     <t>name</t>
   </si>
@@ -221,13 +228,85 @@
     <t>Description_Date</t>
   </si>
   <si>
-    <t>data('Description') + ' @ ' + data('Date_and_Time').toLocaleDateString()</t>
+    <t>query_name</t>
+  </si>
+  <si>
+    <t>query_type</t>
+  </si>
+  <si>
+    <t>linked_form_id</t>
+  </si>
+  <si>
+    <t>linked_table_id</t>
+  </si>
+  <si>
+    <t>selection</t>
+  </si>
+  <si>
+    <t>selectionArgs</t>
+  </si>
+  <si>
+    <t>auxillaryHash</t>
+  </si>
+  <si>
+    <t>linked_table</t>
+  </si>
+  <si>
+    <t>select_geoweather_conditions</t>
+  </si>
+  <si>
+    <t>geoweather_conditions</t>
+  </si>
+  <si>
+    <t>''</t>
+  </si>
+  <si>
+    <t>Language = ?</t>
+  </si>
+  <si>
+    <t>[ 'en' ]</t>
+  </si>
+  <si>
+    <t>data('Description') + ' @ ' + data('Date_and_Time')</t>
+  </si>
+  <si>
+    <t>partition</t>
+  </si>
+  <si>
+    <t>aspect</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>locked</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>filterTypeOnCreation</t>
+  </si>
+  <si>
+    <t>READ_ONLY</t>
+  </si>
+  <si>
+    <t>unverifiedUserCanCreate</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -366,7 +445,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -409,6 +488,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="33">
@@ -451,6 +545,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -780,26 +877,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="8" customWidth="1"/>
     <col min="4" max="5" width="15.6640625" style="11" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="24.5" style="11" customWidth="1"/>
-    <col min="8" max="8" width="42.5" style="7" customWidth="1"/>
-    <col min="9" max="9" width="38.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="24.44140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="42.44140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="38.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22" customHeight="1">
+    <row r="1" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -834,7 +931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>23</v>
       </c>
@@ -855,7 +952,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -869,7 +966,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="13"/>
     </row>
-    <row r="4" spans="1:11" ht="30">
+    <row r="4" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
@@ -881,7 +978,7 @@
       </c>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
@@ -898,12 +995,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.5" customHeight="1">
+    <row r="6" spans="1:11" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>31</v>
@@ -916,7 +1013,7 @@
       </c>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>34</v>
       </c>
@@ -931,7 +1028,7 @@
       </c>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
@@ -949,13 +1046,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="1:11" ht="45">
+    <row r="10" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>23</v>
       </c>
@@ -968,7 +1065,7 @@
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="2"/>
@@ -976,10 +1073,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J12" s="14"/>
     </row>
   </sheetData>
@@ -996,21 +1093,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
+    <col min="2" max="8" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="47.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1021,7 +1271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1029,7 +1279,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1037,7 +1287,7 @@
         <v>20140814</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" customHeight="1">
+    <row r="4" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1295,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1053,7 +1303,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>64</v>
       </c>
@@ -1072,7 +1322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1080,14 +1330,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" customHeight="1">
+    <row r="1" spans="1:3" ht="15.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1098,7 +1348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1109,7 +1359,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1120,7 +1370,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1131,7 +1381,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1142,7 +1392,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1153,7 +1403,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1164,7 +1414,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1175,7 +1425,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Row level access demo changes
</commit_message>
<xml_diff>
--- a/app/config/tables/geoweather/forms/geoweather/geoweather.xlsx
+++ b/app/config/tables/geoweather/forms/geoweather/geoweather.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\geoweather\forms\geoweather\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5446" yWindow="275" windowWidth="25606" windowHeight="16063" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="5440" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -273,9 +268,6 @@
     <t>security</t>
   </si>
   <si>
-    <t>filterTypeOnCreation</t>
-  </si>
-  <si>
     <t>READ_ONLY</t>
   </si>
   <si>
@@ -304,12 +296,15 @@
   </si>
   <si>
     <t>{}</t>
+  </si>
+  <si>
+    <t>defaultAccessOnCreation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -884,22 +879,22 @@
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="8" customWidth="1"/>
     <col min="4" max="5" width="15.6640625" style="11" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="42.44140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="38.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="11" customWidth="1"/>
+    <col min="8" max="8" width="42.5" style="7" customWidth="1"/>
+    <col min="9" max="9" width="38.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" style="5" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.77734375" style="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="22" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -922,19 +917,19 @@
         <v>52</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="B2" s="12" t="s">
         <v>19</v>
       </c>
@@ -955,7 +950,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -969,7 +964,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="13"/>
     </row>
-    <row r="4" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="31.5">
       <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
@@ -981,7 +976,7 @@
       </c>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
@@ -998,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="17.5" customHeight="1">
       <c r="B6" s="8" t="s">
         <v>53</v>
       </c>
@@ -1016,7 +1011,7 @@
       </c>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="B7" s="8" t="s">
         <v>30</v>
       </c>
@@ -1031,7 +1026,7 @@
       </c>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
@@ -1049,13 +1044,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="1:11" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="31.5">
       <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
@@ -1076,10 +1071,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="J12" s="14"/>
     </row>
   </sheetData>
@@ -1098,18 +1093,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -1126,7 +1121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1134,16 +1129,16 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
         <v>79</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1151,16 +1146,16 @@
         <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1174,11 +1169,16 @@
         <v>79</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1190,15 +1190,15 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="6" width="22.77734375" customWidth="1"/>
-    <col min="7" max="7" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="6" width="22.83203125" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" customWidth="1"/>
     <col min="8" max="8" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16.5" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>62</v>
       </c>
@@ -1218,13 +1218,13 @@
         <v>67</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="47.8" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="47.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1244,14 +1244,19 @@
         <v>72</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1263,15 +1268,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.33203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.77734375" style="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1279,10 +1284,10 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1298,7 +1303,7 @@
         <v>20140814</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1306,7 +1311,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1319,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
@@ -1337,18 +1342,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.5" customHeight="1">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1356,10 +1361,10 @@
         <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1370,7 +1375,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1381,7 +1386,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1392,7 +1397,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1403,7 +1408,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1414,7 +1419,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1425,7 +1430,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1436,7 +1441,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>26</v>
       </c>

</xml_diff>